<commit_message>
Now we have custom excel supply.
You still have to make a suitable template, though.
Use %ROW% to mark starting row, and %COL% to mark starting col.
Use DAY MONTH, YEAR to mark the date. It currently supports only one format as shown below.
</commit_message>
<xml_diff>
--- a/library/seat_template.xlsx
+++ b/library/seat_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7cf3a2fcbf616214/文档/Work/seat/library/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="8_{EA047AC3-0F2F-417C-B338-0D97FD44DA34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3EC1395A-741B-406C-A6DC-3D466C2F8A35}"/>
+  <xr:revisionPtr revIDLastSave="66" documentId="8_{EA047AC3-0F2F-417C-B338-0D97FD44DA34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7373338E-BDEA-4784-B132-687D2FDFB490}"/>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="1770" windowWidth="18900" windowHeight="11860" xr2:uid="{34280183-CD2B-44EA-BC63-415E754AED01}"/>
+    <workbookView xWindow="1680" yWindow="2110" windowWidth="18900" windowHeight="11860" xr2:uid="{34280183-CD2B-44EA-BC63-415E754AED01}"/>
   </bookViews>
   <sheets>
     <sheet name="Seats" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>窗户</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -62,6 +62,10 @@
   </si>
   <si>
     <t>ICC S1C5 座位表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$%ROW% %COL%</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -539,20 +543,20 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -871,7 +875,7 @@
   <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+      <selection activeCell="K1" sqref="K1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -894,7 +898,7 @@
       <c r="I1" s="27"/>
       <c r="J1" s="27"/>
       <c r="K1" s="28" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L1" s="28"/>
       <c r="M1" s="29"/>
@@ -914,7 +918,7 @@
       <c r="I2" s="35"/>
       <c r="J2" s="35"/>
       <c r="K2" s="6"/>
-      <c r="L2" s="39" t="s">
+      <c r="L2" s="41" t="s">
         <v>3</v>
       </c>
       <c r="M2" s="9"/>
@@ -934,7 +938,7 @@
       <c r="I3" s="13"/>
       <c r="J3" s="5"/>
       <c r="K3" s="4"/>
-      <c r="L3" s="40"/>
+      <c r="L3" s="42"/>
       <c r="M3" s="10"/>
       <c r="N3" s="3"/>
     </row>
@@ -942,7 +946,9 @@
       <c r="A4" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="14"/>
+      <c r="B4" s="14" t="s">
+        <v>7</v>
+      </c>
       <c r="C4" s="25"/>
       <c r="D4" s="30" t="s">
         <v>5</v>
@@ -975,7 +981,7 @@
       <c r="J5" s="30"/>
       <c r="K5" s="16"/>
       <c r="L5" s="16"/>
-      <c r="M5" s="41" t="s">
+      <c r="M5" s="38" t="s">
         <v>4</v>
       </c>
       <c r="N5" s="3"/>
@@ -993,23 +999,23 @@
       <c r="J6" s="30"/>
       <c r="K6" s="23"/>
       <c r="L6" s="23"/>
-      <c r="M6" s="41"/>
+      <c r="M6" s="38"/>
       <c r="N6" s="3"/>
     </row>
     <row r="7" spans="1:14" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="33"/>
       <c r="B7" s="21"/>
       <c r="C7" s="22"/>
-      <c r="D7" s="38"/>
+      <c r="D7" s="40"/>
       <c r="E7" s="21"/>
       <c r="F7" s="19"/>
       <c r="G7" s="15"/>
       <c r="H7" s="22"/>
       <c r="I7" s="21"/>
-      <c r="J7" s="38"/>
+      <c r="J7" s="40"/>
       <c r="K7" s="24"/>
       <c r="L7" s="19"/>
-      <c r="M7" s="42"/>
+      <c r="M7" s="39"/>
     </row>
     <row r="8" spans="1:14" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>

</xml_diff>